<commit_message>
Add main script file
</commit_message>
<xml_diff>
--- a/Data/excel/Links_To_Modelled_Background_Pollution_Data.xlsx
+++ b/Data/excel/Links_To_Modelled_Background_Pollution_Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-440" windowWidth="25600" windowHeight="20480" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="-435" windowWidth="25605" windowHeight="15990" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -139,6 +139,7 @@
         <sz val="13"/>
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
+        <family val="2"/>
       </rPr>
       <t>2.5</t>
     </r>
@@ -733,12 +734,14 @@
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <vertAlign val="subscript"/>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -752,12 +755,14 @@
       <b/>
       <sz val="13"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -795,6 +800,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1122,19 +1132,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="D73" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="78.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="78.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1154,7 +1164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1174,7 +1184,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1194,7 +1204,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1214,7 +1224,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1234,7 +1244,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1254,7 +1264,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1274,7 +1284,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1294,7 +1304,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1314,7 +1324,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1334,7 +1344,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1354,7 +1364,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1374,7 +1384,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1394,7 +1404,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1411,7 +1421,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1428,7 +1438,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -1445,7 +1455,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1465,7 +1475,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -1485,7 +1495,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -1502,7 +1512,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1519,7 +1529,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1536,7 +1546,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -1553,7 +1563,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -1570,7 +1580,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -1587,7 +1597,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>85</v>
       </c>
@@ -1604,7 +1614,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -1621,7 +1631,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -1638,7 +1648,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -1655,7 +1665,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -1672,7 +1682,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -1689,7 +1699,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -1706,7 +1716,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -1723,7 +1733,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>85</v>
       </c>
@@ -1740,7 +1750,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -1757,7 +1767,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -1774,7 +1784,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -1791,7 +1801,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -1811,7 +1821,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>86</v>
       </c>
@@ -1831,7 +1841,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -1851,7 +1861,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>86</v>
       </c>
@@ -1871,7 +1881,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -1891,7 +1901,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -1911,7 +1921,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -1931,7 +1941,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -1951,7 +1961,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -1971,7 +1981,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -1991,7 +2001,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -2011,7 +2021,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -2031,7 +2041,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>112</v>
       </c>
@@ -2051,7 +2061,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>112</v>
       </c>
@@ -2071,7 +2081,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>112</v>
       </c>
@@ -2091,7 +2101,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>112</v>
       </c>
@@ -2111,7 +2121,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>112</v>
       </c>
@@ -2131,7 +2141,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>112</v>
       </c>
@@ -2151,7 +2161,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>112</v>
       </c>
@@ -2171,7 +2181,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>112</v>
       </c>
@@ -2191,7 +2201,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>112</v>
       </c>
@@ -2211,7 +2221,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -2231,7 +2241,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>112</v>
       </c>
@@ -2251,7 +2261,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>112</v>
       </c>
@@ -2271,7 +2281,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>112</v>
       </c>
@@ -2291,7 +2301,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>112</v>
       </c>
@@ -2311,7 +2321,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>112</v>
       </c>
@@ -2331,7 +2341,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>112</v>
       </c>
@@ -2351,7 +2361,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>112</v>
       </c>
@@ -2371,7 +2381,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>112</v>
       </c>
@@ -2391,7 +2401,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>162</v>
       </c>
@@ -2408,7 +2418,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>162</v>
       </c>
@@ -2425,7 +2435,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>162</v>
       </c>
@@ -2442,7 +2452,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>162</v>
       </c>
@@ -2459,7 +2469,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>162</v>
       </c>
@@ -2476,7 +2486,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>162</v>
       </c>
@@ -2493,7 +2503,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>162</v>
       </c>
@@ -2510,7 +2520,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>162</v>
       </c>
@@ -2527,7 +2537,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>162</v>
       </c>
@@ -2544,7 +2554,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>162</v>
       </c>
@@ -2561,7 +2571,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>162</v>
       </c>
@@ -2578,7 +2588,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>174</v>
       </c>
@@ -2598,7 +2608,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>174</v>
       </c>
@@ -2618,7 +2628,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>174</v>
       </c>
@@ -2638,7 +2648,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>174</v>
       </c>
@@ -2658,7 +2668,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>174</v>
       </c>
@@ -2678,7 +2688,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>174</v>
       </c>
@@ -2698,7 +2708,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>174</v>
       </c>
@@ -2718,7 +2728,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>174</v>
       </c>
@@ -2738,7 +2748,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>174</v>
       </c>
@@ -2758,7 +2768,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>174</v>
       </c>
@@ -2778,7 +2788,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>196</v>
       </c>
@@ -2795,7 +2805,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>196</v>
       </c>
@@ -2812,7 +2822,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>196</v>
       </c>
@@ -2829,7 +2839,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>196</v>
       </c>
@@ -2846,7 +2856,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>196</v>
       </c>
@@ -2863,7 +2873,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>196</v>
       </c>
@@ -2880,7 +2890,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>196</v>
       </c>
@@ -2893,11 +2903,11 @@
       <c r="D94" t="s">
         <v>203</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F94" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>196</v>
       </c>
@@ -2914,7 +2924,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>196</v>
       </c>
@@ -2927,11 +2937,11 @@
       <c r="D96" t="s">
         <v>205</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F96" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>196</v>
       </c>
@@ -2951,6 +2961,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F25" r:id="rId1"/>
+    <hyperlink ref="F96" r:id="rId2"/>
+    <hyperlink ref="F94" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2970,14 +2982,14 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.1640625" customWidth="1"/>
-    <col min="4" max="4" width="89.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.125" customWidth="1"/>
+    <col min="4" max="4" width="89.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17">
+    <row r="1" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2991,7 +3003,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19">
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -3005,7 +3017,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19">
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -3019,7 +3031,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="19">
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
@@ -3033,7 +3045,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="19">
+    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
@@ -3047,7 +3059,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="19">
+    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
@@ -3061,7 +3073,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="19">
+    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -3075,7 +3087,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="19">
+    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>